<commit_message>
aggiunti polifenoli olio 2021
</commit_message>
<xml_diff>
--- a/data-raw/polifenoli/polifenoli_HPLC_olio.xlsx
+++ b/data-raw/polifenoli/polifenoli_HPLC_olio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Desktop\file progetto\polifenoli veri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Desktop\OliveHealthR\data-raw\polifenoli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FA6533-17E4-41A8-8064-BD1A43953E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F801B6-97D9-40F7-A2C0-FA6B0F04A50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="25275" windowHeight="13755" xr2:uid="{D42F1501-9FEC-4851-B7BD-B10C81F9B577}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D42F1501-9FEC-4851-B7BD-B10C81F9B577}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="45">
   <si>
     <t>Idrossitirosolo</t>
   </si>
@@ -170,11 +170,17 @@
   <si>
     <t>CE_02</t>
   </si>
+  <si>
+    <t>AV_04</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,9 +216,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -527,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515717C1-F799-4246-BFAC-63AB3ABCF04F}">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:O136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B73"/>
+      <selection activeCell="A74" sqref="A74:O136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +547,7 @@
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -3981,6 +3988,2967 @@
         <v>3.5539999999999998</v>
       </c>
     </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74" t="s">
+        <v>40</v>
+      </c>
+      <c r="C74" t="s">
+        <v>37</v>
+      </c>
+      <c r="D74">
+        <v>2021</v>
+      </c>
+      <c r="E74" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="G74" s="1">
+        <v>2</v>
+      </c>
+      <c r="H74" s="1">
+        <v>2</v>
+      </c>
+      <c r="I74" s="2">
+        <v>81.251000000000005</v>
+      </c>
+      <c r="J74">
+        <v>67.701999999999998</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="M74">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="N74" s="2">
+        <v>5.734</v>
+      </c>
+      <c r="O74" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75" t="s">
+        <v>40</v>
+      </c>
+      <c r="C75" t="s">
+        <v>37</v>
+      </c>
+      <c r="D75">
+        <v>2021</v>
+      </c>
+      <c r="E75" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75" s="1">
+        <v>2</v>
+      </c>
+      <c r="H75" s="1">
+        <v>2</v>
+      </c>
+      <c r="I75" s="2">
+        <v>78.989000000000004</v>
+      </c>
+      <c r="J75">
+        <v>67.251000000000005</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="M75">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="N75">
+        <v>6.2149999999999999</v>
+      </c>
+      <c r="O75" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>11</v>
+      </c>
+      <c r="B76" t="s">
+        <v>40</v>
+      </c>
+      <c r="C76" t="s">
+        <v>37</v>
+      </c>
+      <c r="D76">
+        <v>2021</v>
+      </c>
+      <c r="E76" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="G76" s="1">
+        <v>2</v>
+      </c>
+      <c r="H76" s="1">
+        <v>2</v>
+      </c>
+      <c r="I76" s="2">
+        <v>79.054000000000002</v>
+      </c>
+      <c r="J76">
+        <v>68.203000000000003</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="M76">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="N76">
+        <v>5.891</v>
+      </c>
+      <c r="O76" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" t="s">
+        <v>40</v>
+      </c>
+      <c r="C77" t="s">
+        <v>37</v>
+      </c>
+      <c r="D77">
+        <v>2021</v>
+      </c>
+      <c r="E77" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77" s="1">
+        <v>2</v>
+      </c>
+      <c r="H77" s="1">
+        <v>2</v>
+      </c>
+      <c r="I77" s="2">
+        <v>104.69</v>
+      </c>
+      <c r="J77">
+        <v>55.131999999999998</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="L77">
+        <v>1.292</v>
+      </c>
+      <c r="M77">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="N77">
+        <v>165.73099999999999</v>
+      </c>
+      <c r="O77" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" t="s">
+        <v>40</v>
+      </c>
+      <c r="C78" t="s">
+        <v>37</v>
+      </c>
+      <c r="D78">
+        <v>2021</v>
+      </c>
+      <c r="E78" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78" s="1">
+        <v>2</v>
+      </c>
+      <c r="H78" s="1">
+        <v>2</v>
+      </c>
+      <c r="I78" s="2">
+        <v>105.23</v>
+      </c>
+      <c r="J78">
+        <v>55.222000000000001</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>1.325</v>
+      </c>
+      <c r="M78">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="N78">
+        <v>164.22900000000001</v>
+      </c>
+      <c r="O78" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" t="s">
+        <v>40</v>
+      </c>
+      <c r="C79" t="s">
+        <v>37</v>
+      </c>
+      <c r="D79">
+        <v>2021</v>
+      </c>
+      <c r="E79" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79" s="1">
+        <v>2</v>
+      </c>
+      <c r="H79" s="1">
+        <v>2</v>
+      </c>
+      <c r="I79" s="2">
+        <v>203.95599999999999</v>
+      </c>
+      <c r="J79">
+        <v>54.238</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>1.2769999999999999</v>
+      </c>
+      <c r="M79">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="N79">
+        <v>167.297</v>
+      </c>
+      <c r="O79" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>13</v>
+      </c>
+      <c r="B80" t="s">
+        <v>40</v>
+      </c>
+      <c r="C80" t="s">
+        <v>37</v>
+      </c>
+      <c r="D80">
+        <v>2021</v>
+      </c>
+      <c r="E80" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80" s="1">
+        <v>2</v>
+      </c>
+      <c r="H80" s="1">
+        <v>2</v>
+      </c>
+      <c r="I80" s="2">
+        <v>76.122</v>
+      </c>
+      <c r="J80">
+        <v>58.143000000000001</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>1.2010000000000001</v>
+      </c>
+      <c r="M80">
+        <v>3.726</v>
+      </c>
+      <c r="N80">
+        <v>191.73500000000001</v>
+      </c>
+      <c r="O80" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81" t="s">
+        <v>40</v>
+      </c>
+      <c r="C81" t="s">
+        <v>37</v>
+      </c>
+      <c r="D81">
+        <v>2021</v>
+      </c>
+      <c r="E81" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81" s="1">
+        <v>2</v>
+      </c>
+      <c r="H81" s="1">
+        <v>2</v>
+      </c>
+      <c r="I81" s="2">
+        <v>77.337999999999994</v>
+      </c>
+      <c r="J81">
+        <v>57.264000000000003</v>
+      </c>
+      <c r="K81">
+        <v>0.123</v>
+      </c>
+      <c r="L81">
+        <v>1.3009999999999999</v>
+      </c>
+      <c r="M81">
+        <v>3.8639999999999999</v>
+      </c>
+      <c r="N81">
+        <v>202.56700000000001</v>
+      </c>
+      <c r="O81" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>13</v>
+      </c>
+      <c r="B82" t="s">
+        <v>40</v>
+      </c>
+      <c r="C82" t="s">
+        <v>37</v>
+      </c>
+      <c r="D82">
+        <v>2021</v>
+      </c>
+      <c r="E82" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82" s="1">
+        <v>2</v>
+      </c>
+      <c r="H82" s="1">
+        <v>2</v>
+      </c>
+      <c r="I82" s="2">
+        <v>76.826999999999998</v>
+      </c>
+      <c r="J82">
+        <v>58.642000000000003</v>
+      </c>
+      <c r="K82">
+        <v>0.15</v>
+      </c>
+      <c r="L82">
+        <v>1.258</v>
+      </c>
+      <c r="M82">
+        <v>3.6869999999999998</v>
+      </c>
+      <c r="N82">
+        <v>190.56200000000001</v>
+      </c>
+      <c r="O82" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>44</v>
+      </c>
+      <c r="B83" t="s">
+        <v>40</v>
+      </c>
+      <c r="C83" t="s">
+        <v>37</v>
+      </c>
+      <c r="D83">
+        <v>2021</v>
+      </c>
+      <c r="E83" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="G83" s="1">
+        <v>2</v>
+      </c>
+      <c r="H83" s="1">
+        <v>2</v>
+      </c>
+      <c r="I83" s="2">
+        <v>74.534999999999997</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="M83">
+        <v>1.9650000000000001</v>
+      </c>
+      <c r="N83">
+        <v>54.654000000000003</v>
+      </c>
+      <c r="O83" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>44</v>
+      </c>
+      <c r="B84" t="s">
+        <v>40</v>
+      </c>
+      <c r="C84" t="s">
+        <v>37</v>
+      </c>
+      <c r="D84">
+        <v>2021</v>
+      </c>
+      <c r="E84" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84" s="1">
+        <v>2</v>
+      </c>
+      <c r="H84" s="1">
+        <v>2</v>
+      </c>
+      <c r="I84" s="2">
+        <v>75.364000000000004</v>
+      </c>
+      <c r="J84">
+        <v>0.159</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="M84">
+        <v>2.016</v>
+      </c>
+      <c r="N84">
+        <v>55.267000000000003</v>
+      </c>
+      <c r="O84" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>44</v>
+      </c>
+      <c r="B85" t="s">
+        <v>40</v>
+      </c>
+      <c r="C85" t="s">
+        <v>37</v>
+      </c>
+      <c r="D85">
+        <v>2021</v>
+      </c>
+      <c r="E85" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="G85" s="1">
+        <v>2</v>
+      </c>
+      <c r="H85" s="1">
+        <v>2</v>
+      </c>
+      <c r="I85" s="2">
+        <v>74.923000000000002</v>
+      </c>
+      <c r="J85">
+        <v>0.124</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="M85">
+        <v>1.9990000000000001</v>
+      </c>
+      <c r="N85">
+        <v>56.87</v>
+      </c>
+      <c r="O85" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>15</v>
+      </c>
+      <c r="B86" t="s">
+        <v>40</v>
+      </c>
+      <c r="C86" t="s">
+        <v>37</v>
+      </c>
+      <c r="D86">
+        <v>2021</v>
+      </c>
+      <c r="E86" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86" s="1">
+        <v>2</v>
+      </c>
+      <c r="H86" s="1">
+        <v>2</v>
+      </c>
+      <c r="I86" s="2">
+        <v>60.046999999999997</v>
+      </c>
+      <c r="J86">
+        <v>65.328999999999994</v>
+      </c>
+      <c r="K86">
+        <v>13.679</v>
+      </c>
+      <c r="L86">
+        <v>1.2909999999999999</v>
+      </c>
+      <c r="M86">
+        <v>3.8140000000000001</v>
+      </c>
+      <c r="N86">
+        <v>21.28</v>
+      </c>
+      <c r="O86" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>15</v>
+      </c>
+      <c r="B87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C87" t="s">
+        <v>37</v>
+      </c>
+      <c r="D87">
+        <v>2021</v>
+      </c>
+      <c r="E87" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87" s="1">
+        <v>2</v>
+      </c>
+      <c r="H87" s="1">
+        <v>2</v>
+      </c>
+      <c r="I87" s="2">
+        <v>62.588999999999999</v>
+      </c>
+      <c r="J87">
+        <v>66.238</v>
+      </c>
+      <c r="K87">
+        <v>12.987</v>
+      </c>
+      <c r="L87">
+        <v>1.302</v>
+      </c>
+      <c r="M87">
+        <v>4.532</v>
+      </c>
+      <c r="N87">
+        <v>22.312000000000001</v>
+      </c>
+      <c r="O87" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>15</v>
+      </c>
+      <c r="B88" t="s">
+        <v>40</v>
+      </c>
+      <c r="C88" t="s">
+        <v>37</v>
+      </c>
+      <c r="D88">
+        <v>2021</v>
+      </c>
+      <c r="E88" t="s">
+        <v>10</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88" s="1">
+        <v>2</v>
+      </c>
+      <c r="H88" s="1">
+        <v>2</v>
+      </c>
+      <c r="I88" s="2">
+        <v>61.555</v>
+      </c>
+      <c r="J88">
+        <v>67.891000000000005</v>
+      </c>
+      <c r="K88">
+        <v>13.118</v>
+      </c>
+      <c r="L88">
+        <v>1.119</v>
+      </c>
+      <c r="M88">
+        <v>3.9119999999999999</v>
+      </c>
+      <c r="N88">
+        <v>20.937000000000001</v>
+      </c>
+      <c r="O88" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B89" t="s">
+        <v>40</v>
+      </c>
+      <c r="C89" t="s">
+        <v>37</v>
+      </c>
+      <c r="D89">
+        <v>2021</v>
+      </c>
+      <c r="E89" t="s">
+        <v>8</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="G89" s="1">
+        <v>2</v>
+      </c>
+      <c r="H89" s="1">
+        <v>2</v>
+      </c>
+      <c r="I89" s="2">
+        <v>54.070999999999998</v>
+      </c>
+      <c r="J89">
+        <v>55.91</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="L89">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="M89">
+        <v>1.1020000000000001</v>
+      </c>
+      <c r="N89">
+        <v>43.777000000000001</v>
+      </c>
+      <c r="O89" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>16</v>
+      </c>
+      <c r="B90" t="s">
+        <v>40</v>
+      </c>
+      <c r="C90" t="s">
+        <v>37</v>
+      </c>
+      <c r="D90">
+        <v>2021</v>
+      </c>
+      <c r="E90" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90" s="1">
+        <v>2</v>
+      </c>
+      <c r="H90" s="1">
+        <v>2</v>
+      </c>
+      <c r="I90" s="2">
+        <v>55.234999999999999</v>
+      </c>
+      <c r="J90">
+        <v>55.197000000000003</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+      <c r="L90">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="M90">
+        <v>1.1180000000000001</v>
+      </c>
+      <c r="N90">
+        <v>43.831000000000003</v>
+      </c>
+      <c r="O90" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>16</v>
+      </c>
+      <c r="B91" t="s">
+        <v>40</v>
+      </c>
+      <c r="C91" t="s">
+        <v>37</v>
+      </c>
+      <c r="D91">
+        <v>2021</v>
+      </c>
+      <c r="E91" t="s">
+        <v>10</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="G91" s="1">
+        <v>2</v>
+      </c>
+      <c r="H91" s="1">
+        <v>2</v>
+      </c>
+      <c r="I91" s="2">
+        <v>54.902999999999999</v>
+      </c>
+      <c r="J91">
+        <v>54.265000000000001</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="L91">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="M91">
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="N91">
+        <v>44.87</v>
+      </c>
+      <c r="O91" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92" t="s">
+        <v>40</v>
+      </c>
+      <c r="C92" t="s">
+        <v>37</v>
+      </c>
+      <c r="D92">
+        <v>2021</v>
+      </c>
+      <c r="E92" t="s">
+        <v>8</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92" s="1">
+        <v>2</v>
+      </c>
+      <c r="H92" s="1">
+        <v>2</v>
+      </c>
+      <c r="I92" s="2">
+        <v>65.364999999999995</v>
+      </c>
+      <c r="J92">
+        <v>61.24</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+      <c r="L92">
+        <v>1.0589999999999999</v>
+      </c>
+      <c r="M92">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="N92">
+        <v>28.725000000000001</v>
+      </c>
+      <c r="O92" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>17</v>
+      </c>
+      <c r="B93" t="s">
+        <v>40</v>
+      </c>
+      <c r="C93" t="s">
+        <v>37</v>
+      </c>
+      <c r="D93">
+        <v>2021</v>
+      </c>
+      <c r="E93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93" s="1">
+        <v>2</v>
+      </c>
+      <c r="H93" s="1">
+        <v>2</v>
+      </c>
+      <c r="I93" s="2">
+        <v>66.587000000000003</v>
+      </c>
+      <c r="J93">
+        <v>62.097999999999999</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="M93">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="N93">
+        <v>30.571000000000002</v>
+      </c>
+      <c r="O93" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>17</v>
+      </c>
+      <c r="B94" t="s">
+        <v>40</v>
+      </c>
+      <c r="C94" t="s">
+        <v>37</v>
+      </c>
+      <c r="D94">
+        <v>2021</v>
+      </c>
+      <c r="E94" t="s">
+        <v>10</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94" s="1">
+        <v>2</v>
+      </c>
+      <c r="H94" s="1">
+        <v>2</v>
+      </c>
+      <c r="I94" s="2">
+        <v>64.238</v>
+      </c>
+      <c r="J94">
+        <v>60.521999999999998</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+      <c r="L94">
+        <v>1.125</v>
+      </c>
+      <c r="M94">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="N94">
+        <v>29.332999999999998</v>
+      </c>
+      <c r="O94" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B95" t="s">
+        <v>40</v>
+      </c>
+      <c r="C95" t="s">
+        <v>37</v>
+      </c>
+      <c r="D95">
+        <v>2021</v>
+      </c>
+      <c r="E95" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
+      </c>
+      <c r="G95" s="1">
+        <v>2</v>
+      </c>
+      <c r="H95" s="1">
+        <v>2</v>
+      </c>
+      <c r="I95" s="2">
+        <v>75.819000000000003</v>
+      </c>
+      <c r="J95">
+        <v>65.608999999999995</v>
+      </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="L95">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="M95">
+        <v>3.2850000000000001</v>
+      </c>
+      <c r="N95">
+        <v>22.544</v>
+      </c>
+      <c r="O95" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>18</v>
+      </c>
+      <c r="B96" t="s">
+        <v>40</v>
+      </c>
+      <c r="C96" t="s">
+        <v>37</v>
+      </c>
+      <c r="D96">
+        <v>2021</v>
+      </c>
+      <c r="E96" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
+      </c>
+      <c r="G96" s="1">
+        <v>2</v>
+      </c>
+      <c r="H96" s="1">
+        <v>2</v>
+      </c>
+      <c r="I96" s="2">
+        <v>77.686999999999998</v>
+      </c>
+      <c r="J96">
+        <v>65.272000000000006</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="M96">
+        <v>3.1579999999999999</v>
+      </c>
+      <c r="N96">
+        <v>22.873000000000001</v>
+      </c>
+      <c r="O96" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>18</v>
+      </c>
+      <c r="B97" t="s">
+        <v>40</v>
+      </c>
+      <c r="C97" t="s">
+        <v>37</v>
+      </c>
+      <c r="D97">
+        <v>2021</v>
+      </c>
+      <c r="E97" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97">
+        <v>1</v>
+      </c>
+      <c r="G97" s="1">
+        <v>2</v>
+      </c>
+      <c r="H97" s="1">
+        <v>2</v>
+      </c>
+      <c r="I97" s="2">
+        <v>74.221999999999994</v>
+      </c>
+      <c r="J97">
+        <v>66.578000000000003</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="M97">
+        <v>3.331</v>
+      </c>
+      <c r="N97">
+        <v>21.891999999999999</v>
+      </c>
+      <c r="O97" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>19</v>
+      </c>
+      <c r="B98" t="s">
+        <v>40</v>
+      </c>
+      <c r="C98" t="s">
+        <v>37</v>
+      </c>
+      <c r="D98">
+        <v>2021</v>
+      </c>
+      <c r="E98" t="s">
+        <v>8</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98" s="1">
+        <v>2</v>
+      </c>
+      <c r="H98" s="1">
+        <v>2</v>
+      </c>
+      <c r="I98" s="2">
+        <v>44.927</v>
+      </c>
+      <c r="J98">
+        <v>75.287000000000006</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>2.274</v>
+      </c>
+      <c r="M98">
+        <v>3.512</v>
+      </c>
+      <c r="N98">
+        <v>49.23</v>
+      </c>
+      <c r="O98" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>19</v>
+      </c>
+      <c r="B99" t="s">
+        <v>40</v>
+      </c>
+      <c r="C99" t="s">
+        <v>37</v>
+      </c>
+      <c r="D99">
+        <v>2021</v>
+      </c>
+      <c r="E99" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99" s="1">
+        <v>2</v>
+      </c>
+      <c r="H99" s="1">
+        <v>2</v>
+      </c>
+      <c r="I99" s="2">
+        <v>45.234999999999999</v>
+      </c>
+      <c r="J99">
+        <v>75.335999999999999</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>2.1379999999999999</v>
+      </c>
+      <c r="M99">
+        <v>3.6779999999999999</v>
+      </c>
+      <c r="N99">
+        <v>50.332999999999998</v>
+      </c>
+      <c r="O99" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>19</v>
+      </c>
+      <c r="B100" t="s">
+        <v>40</v>
+      </c>
+      <c r="C100" t="s">
+        <v>37</v>
+      </c>
+      <c r="D100">
+        <v>2021</v>
+      </c>
+      <c r="E100" t="s">
+        <v>10</v>
+      </c>
+      <c r="F100">
+        <v>1</v>
+      </c>
+      <c r="G100" s="1">
+        <v>2</v>
+      </c>
+      <c r="H100" s="1">
+        <v>2</v>
+      </c>
+      <c r="I100" s="2">
+        <v>44.792000000000002</v>
+      </c>
+      <c r="J100">
+        <v>77.257999999999996</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <v>1.9870000000000001</v>
+      </c>
+      <c r="M100">
+        <v>3.5550000000000002</v>
+      </c>
+      <c r="N100">
+        <v>51.289000000000001</v>
+      </c>
+      <c r="O100" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>20</v>
+      </c>
+      <c r="B101" t="s">
+        <v>40</v>
+      </c>
+      <c r="C101" t="s">
+        <v>37</v>
+      </c>
+      <c r="D101">
+        <v>2021</v>
+      </c>
+      <c r="E101" t="s">
+        <v>8</v>
+      </c>
+      <c r="F101">
+        <v>1</v>
+      </c>
+      <c r="G101" s="1">
+        <v>2</v>
+      </c>
+      <c r="H101" s="1">
+        <v>2</v>
+      </c>
+      <c r="I101" s="2">
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>59.887</v>
+      </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
+      <c r="L101">
+        <v>0.79</v>
+      </c>
+      <c r="M101">
+        <v>2.012</v>
+      </c>
+      <c r="N101">
+        <v>42.537999999999997</v>
+      </c>
+      <c r="O101" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>20</v>
+      </c>
+      <c r="B102" t="s">
+        <v>40</v>
+      </c>
+      <c r="C102" t="s">
+        <v>37</v>
+      </c>
+      <c r="D102">
+        <v>2021</v>
+      </c>
+      <c r="E102" t="s">
+        <v>9</v>
+      </c>
+      <c r="F102">
+        <v>1</v>
+      </c>
+      <c r="G102" s="1">
+        <v>2</v>
+      </c>
+      <c r="H102" s="1">
+        <v>2</v>
+      </c>
+      <c r="I102" s="2">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="J102">
+        <v>62.351999999999997</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="M102">
+        <v>2.1579999999999999</v>
+      </c>
+      <c r="N102">
+        <v>41.662999999999997</v>
+      </c>
+      <c r="O102" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>20</v>
+      </c>
+      <c r="B103" t="s">
+        <v>40</v>
+      </c>
+      <c r="C103" t="s">
+        <v>37</v>
+      </c>
+      <c r="D103">
+        <v>2021</v>
+      </c>
+      <c r="E103" t="s">
+        <v>10</v>
+      </c>
+      <c r="F103">
+        <v>1</v>
+      </c>
+      <c r="G103" s="1">
+        <v>2</v>
+      </c>
+      <c r="H103" s="1">
+        <v>2</v>
+      </c>
+      <c r="I103" s="2">
+        <v>0.111</v>
+      </c>
+      <c r="J103">
+        <v>69.933999999999997</v>
+      </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
+      <c r="L103">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="M103">
+        <v>2.222</v>
+      </c>
+      <c r="N103">
+        <v>43.677999999999997</v>
+      </c>
+      <c r="O103" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>21</v>
+      </c>
+      <c r="B104" t="s">
+        <v>40</v>
+      </c>
+      <c r="C104" t="s">
+        <v>37</v>
+      </c>
+      <c r="D104">
+        <v>2021</v>
+      </c>
+      <c r="E104" t="s">
+        <v>8</v>
+      </c>
+      <c r="F104">
+        <v>1</v>
+      </c>
+      <c r="G104" s="1">
+        <v>2</v>
+      </c>
+      <c r="H104" s="1">
+        <v>2</v>
+      </c>
+      <c r="I104" s="2">
+        <v>0</v>
+      </c>
+      <c r="J104">
+        <v>78.738</v>
+      </c>
+      <c r="K104">
+        <v>33.607999999999997</v>
+      </c>
+      <c r="L104">
+        <v>3.7709999999999999</v>
+      </c>
+      <c r="M104">
+        <v>1.373</v>
+      </c>
+      <c r="N104">
+        <v>54.883000000000003</v>
+      </c>
+      <c r="O104" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>21</v>
+      </c>
+      <c r="B105" t="s">
+        <v>40</v>
+      </c>
+      <c r="C105" t="s">
+        <v>37</v>
+      </c>
+      <c r="D105">
+        <v>2021</v>
+      </c>
+      <c r="E105" t="s">
+        <v>9</v>
+      </c>
+      <c r="F105">
+        <v>1</v>
+      </c>
+      <c r="G105" s="1">
+        <v>2</v>
+      </c>
+      <c r="H105" s="1">
+        <v>2</v>
+      </c>
+      <c r="I105" s="2">
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>79.225999999999999</v>
+      </c>
+      <c r="K105">
+        <v>34.222000000000001</v>
+      </c>
+      <c r="L105">
+        <v>4.1280000000000001</v>
+      </c>
+      <c r="M105">
+        <v>1.444</v>
+      </c>
+      <c r="N105">
+        <v>55.094000000000001</v>
+      </c>
+      <c r="O105" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>21</v>
+      </c>
+      <c r="B106" t="s">
+        <v>40</v>
+      </c>
+      <c r="C106" t="s">
+        <v>37</v>
+      </c>
+      <c r="D106">
+        <v>2021</v>
+      </c>
+      <c r="E106" t="s">
+        <v>10</v>
+      </c>
+      <c r="F106">
+        <v>1</v>
+      </c>
+      <c r="G106" s="1">
+        <v>2</v>
+      </c>
+      <c r="H106" s="1">
+        <v>2</v>
+      </c>
+      <c r="I106" s="2">
+        <v>0</v>
+      </c>
+      <c r="J106">
+        <v>77.555000000000007</v>
+      </c>
+      <c r="K106">
+        <v>35.277999999999999</v>
+      </c>
+      <c r="L106">
+        <v>3.9049999999999998</v>
+      </c>
+      <c r="M106">
+        <v>1.0589999999999999</v>
+      </c>
+      <c r="N106">
+        <v>54.000999999999998</v>
+      </c>
+      <c r="O106" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>22</v>
+      </c>
+      <c r="B107" t="s">
+        <v>40</v>
+      </c>
+      <c r="C107" t="s">
+        <v>37</v>
+      </c>
+      <c r="D107">
+        <v>2021</v>
+      </c>
+      <c r="E107" t="s">
+        <v>8</v>
+      </c>
+      <c r="F107">
+        <v>1</v>
+      </c>
+      <c r="G107" s="1">
+        <v>2</v>
+      </c>
+      <c r="H107" s="1">
+        <v>2</v>
+      </c>
+      <c r="I107" s="2">
+        <v>46.015999999999998</v>
+      </c>
+      <c r="J107">
+        <v>63.725000000000001</v>
+      </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
+      <c r="L107">
+        <v>1.669</v>
+      </c>
+      <c r="M107">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="N107">
+        <v>37.792000000000002</v>
+      </c>
+      <c r="O107" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>22</v>
+      </c>
+      <c r="B108" t="s">
+        <v>40</v>
+      </c>
+      <c r="C108" t="s">
+        <v>37</v>
+      </c>
+      <c r="D108">
+        <v>2021</v>
+      </c>
+      <c r="E108" t="s">
+        <v>9</v>
+      </c>
+      <c r="F108">
+        <v>1</v>
+      </c>
+      <c r="G108" s="1">
+        <v>2</v>
+      </c>
+      <c r="H108" s="1">
+        <v>2</v>
+      </c>
+      <c r="I108" s="2">
+        <v>45.125999999999998</v>
+      </c>
+      <c r="J108">
+        <v>65.238</v>
+      </c>
+      <c r="K108">
+        <v>0</v>
+      </c>
+      <c r="L108">
+        <v>1.7829999999999999</v>
+      </c>
+      <c r="M108">
+        <v>0.879</v>
+      </c>
+      <c r="N108">
+        <v>35.665999999999997</v>
+      </c>
+      <c r="O108" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>42</v>
+      </c>
+      <c r="B109" t="s">
+        <v>40</v>
+      </c>
+      <c r="C109" t="s">
+        <v>37</v>
+      </c>
+      <c r="D109">
+        <v>2021</v>
+      </c>
+      <c r="E109" t="s">
+        <v>10</v>
+      </c>
+      <c r="F109">
+        <v>1</v>
+      </c>
+      <c r="G109" s="1">
+        <v>2</v>
+      </c>
+      <c r="H109" s="1">
+        <v>2</v>
+      </c>
+      <c r="I109" s="2">
+        <v>46.387</v>
+      </c>
+      <c r="J109">
+        <v>63.396999999999998</v>
+      </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
+      <c r="L109">
+        <v>1.726</v>
+      </c>
+      <c r="M109">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="N109">
+        <v>37.097999999999999</v>
+      </c>
+      <c r="O109" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>23</v>
+      </c>
+      <c r="B110" t="s">
+        <v>40</v>
+      </c>
+      <c r="C110" t="s">
+        <v>37</v>
+      </c>
+      <c r="D110">
+        <v>2021</v>
+      </c>
+      <c r="E110" t="s">
+        <v>8</v>
+      </c>
+      <c r="F110">
+        <v>1</v>
+      </c>
+      <c r="G110" s="1">
+        <v>2</v>
+      </c>
+      <c r="H110" s="1">
+        <v>2</v>
+      </c>
+      <c r="I110" s="2">
+        <v>13.907999999999999</v>
+      </c>
+      <c r="J110">
+        <v>47.965000000000003</v>
+      </c>
+      <c r="K110">
+        <v>0</v>
+      </c>
+      <c r="L110">
+        <v>1.1779999999999999</v>
+      </c>
+      <c r="M110">
+        <v>0</v>
+      </c>
+      <c r="N110">
+        <v>19.501999999999999</v>
+      </c>
+      <c r="O110" s="2">
+        <v>4.5410000000000004</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>23</v>
+      </c>
+      <c r="B111" t="s">
+        <v>40</v>
+      </c>
+      <c r="C111" t="s">
+        <v>37</v>
+      </c>
+      <c r="D111">
+        <v>2021</v>
+      </c>
+      <c r="E111" t="s">
+        <v>9</v>
+      </c>
+      <c r="F111">
+        <v>1</v>
+      </c>
+      <c r="G111" s="1">
+        <v>2</v>
+      </c>
+      <c r="H111" s="1">
+        <v>2</v>
+      </c>
+      <c r="I111" s="2">
+        <v>14.234999999999999</v>
+      </c>
+      <c r="J111">
+        <v>48.253999999999998</v>
+      </c>
+      <c r="K111">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="L111">
+        <v>1.2010000000000001</v>
+      </c>
+      <c r="M111">
+        <v>0</v>
+      </c>
+      <c r="N111">
+        <v>20.135000000000002</v>
+      </c>
+      <c r="O111" s="2">
+        <v>4.2149999999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" t="s">
+        <v>40</v>
+      </c>
+      <c r="C112" t="s">
+        <v>37</v>
+      </c>
+      <c r="D112">
+        <v>2021</v>
+      </c>
+      <c r="E112" t="s">
+        <v>10</v>
+      </c>
+      <c r="F112">
+        <v>1</v>
+      </c>
+      <c r="G112" s="1">
+        <v>2</v>
+      </c>
+      <c r="H112" s="1">
+        <v>2</v>
+      </c>
+      <c r="I112" s="2">
+        <v>14.864000000000001</v>
+      </c>
+      <c r="J112">
+        <v>45.368000000000002</v>
+      </c>
+      <c r="K112">
+        <v>0.125</v>
+      </c>
+      <c r="L112">
+        <v>1.196</v>
+      </c>
+      <c r="M112">
+        <v>0</v>
+      </c>
+      <c r="N112">
+        <v>21.227</v>
+      </c>
+      <c r="O112" s="2">
+        <v>3.9510000000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>24</v>
+      </c>
+      <c r="B113" t="s">
+        <v>40</v>
+      </c>
+      <c r="C113" t="s">
+        <v>37</v>
+      </c>
+      <c r="D113">
+        <v>2021</v>
+      </c>
+      <c r="E113" t="s">
+        <v>8</v>
+      </c>
+      <c r="F113">
+        <v>1</v>
+      </c>
+      <c r="G113" s="1">
+        <v>2</v>
+      </c>
+      <c r="H113" s="1">
+        <v>2</v>
+      </c>
+      <c r="I113" s="2">
+        <v>20.593</v>
+      </c>
+      <c r="J113">
+        <v>71.311000000000007</v>
+      </c>
+      <c r="K113">
+        <v>2.3879999999999999</v>
+      </c>
+      <c r="L113">
+        <v>1.92</v>
+      </c>
+      <c r="M113">
+        <v>1.1559999999999999</v>
+      </c>
+      <c r="N113">
+        <v>16.597999999999999</v>
+      </c>
+      <c r="O113" s="2">
+        <v>20.516999999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>24</v>
+      </c>
+      <c r="B114" t="s">
+        <v>40</v>
+      </c>
+      <c r="C114" t="s">
+        <v>37</v>
+      </c>
+      <c r="D114">
+        <v>2021</v>
+      </c>
+      <c r="E114" t="s">
+        <v>9</v>
+      </c>
+      <c r="F114">
+        <v>1</v>
+      </c>
+      <c r="G114" s="1">
+        <v>2</v>
+      </c>
+      <c r="H114" s="1">
+        <v>2</v>
+      </c>
+      <c r="I114" s="2">
+        <v>21.335999999999999</v>
+      </c>
+      <c r="J114">
+        <v>72.665999999999997</v>
+      </c>
+      <c r="K114">
+        <v>3.012</v>
+      </c>
+      <c r="L114">
+        <v>2.1560000000000001</v>
+      </c>
+      <c r="M114">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="N114">
+        <v>18.222000000000001</v>
+      </c>
+      <c r="O114" s="2">
+        <v>19.521000000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>24</v>
+      </c>
+      <c r="B115" t="s">
+        <v>40</v>
+      </c>
+      <c r="C115" t="s">
+        <v>37</v>
+      </c>
+      <c r="D115">
+        <v>2021</v>
+      </c>
+      <c r="E115" t="s">
+        <v>10</v>
+      </c>
+      <c r="F115">
+        <v>1</v>
+      </c>
+      <c r="G115" s="1">
+        <v>2</v>
+      </c>
+      <c r="H115" s="1">
+        <v>2</v>
+      </c>
+      <c r="I115" s="2">
+        <v>20.706</v>
+      </c>
+      <c r="J115">
+        <v>70.566999999999993</v>
+      </c>
+      <c r="K115">
+        <v>2.4319999999999999</v>
+      </c>
+      <c r="L115">
+        <v>1.5760000000000001</v>
+      </c>
+      <c r="M115">
+        <v>1.179</v>
+      </c>
+      <c r="N115">
+        <v>17.597999999999999</v>
+      </c>
+      <c r="O115" s="2">
+        <v>17.667000000000002</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>41</v>
+      </c>
+      <c r="B116" t="s">
+        <v>40</v>
+      </c>
+      <c r="C116" t="s">
+        <v>37</v>
+      </c>
+      <c r="D116">
+        <v>2021</v>
+      </c>
+      <c r="E116" t="s">
+        <v>8</v>
+      </c>
+      <c r="F116">
+        <v>1</v>
+      </c>
+      <c r="G116" s="1">
+        <v>2</v>
+      </c>
+      <c r="H116" s="1">
+        <v>2</v>
+      </c>
+      <c r="I116" s="2">
+        <v>55.451000000000001</v>
+      </c>
+      <c r="J116">
+        <v>0</v>
+      </c>
+      <c r="K116">
+        <v>0</v>
+      </c>
+      <c r="L116">
+        <v>1.3120000000000001</v>
+      </c>
+      <c r="M116">
+        <v>4.4610000000000003</v>
+      </c>
+      <c r="N116">
+        <v>23.117999999999999</v>
+      </c>
+      <c r="O116" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>41</v>
+      </c>
+      <c r="B117" t="s">
+        <v>40</v>
+      </c>
+      <c r="C117" t="s">
+        <v>37</v>
+      </c>
+      <c r="D117">
+        <v>2021</v>
+      </c>
+      <c r="E117" t="s">
+        <v>9</v>
+      </c>
+      <c r="F117">
+        <v>1</v>
+      </c>
+      <c r="G117" s="1">
+        <v>2</v>
+      </c>
+      <c r="H117" s="1">
+        <v>2</v>
+      </c>
+      <c r="I117" s="2">
+        <v>54.125999999999998</v>
+      </c>
+      <c r="J117">
+        <v>0</v>
+      </c>
+      <c r="K117">
+        <v>0</v>
+      </c>
+      <c r="L117">
+        <v>1.444</v>
+      </c>
+      <c r="M117">
+        <v>4.952</v>
+      </c>
+      <c r="N117">
+        <v>23.024000000000001</v>
+      </c>
+      <c r="O117" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>41</v>
+      </c>
+      <c r="B118" t="s">
+        <v>40</v>
+      </c>
+      <c r="C118" t="s">
+        <v>37</v>
+      </c>
+      <c r="D118">
+        <v>2021</v>
+      </c>
+      <c r="E118" t="s">
+        <v>10</v>
+      </c>
+      <c r="F118">
+        <v>1</v>
+      </c>
+      <c r="G118" s="1">
+        <v>2</v>
+      </c>
+      <c r="H118" s="1">
+        <v>2</v>
+      </c>
+      <c r="I118" s="2">
+        <v>55.972000000000001</v>
+      </c>
+      <c r="J118">
+        <v>0</v>
+      </c>
+      <c r="K118">
+        <v>0</v>
+      </c>
+      <c r="L118">
+        <v>1.524</v>
+      </c>
+      <c r="M118">
+        <v>1.4019999999999999</v>
+      </c>
+      <c r="N118">
+        <v>22.986999999999998</v>
+      </c>
+      <c r="O118" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>25</v>
+      </c>
+      <c r="B119" t="s">
+        <v>40</v>
+      </c>
+      <c r="C119" t="s">
+        <v>37</v>
+      </c>
+      <c r="D119">
+        <v>2021</v>
+      </c>
+      <c r="E119" t="s">
+        <v>8</v>
+      </c>
+      <c r="F119">
+        <v>1</v>
+      </c>
+      <c r="G119" s="1">
+        <v>2</v>
+      </c>
+      <c r="H119" s="1">
+        <v>2</v>
+      </c>
+      <c r="I119" s="2">
+        <v>40.786000000000001</v>
+      </c>
+      <c r="J119">
+        <v>54.06</v>
+      </c>
+      <c r="K119">
+        <v>0</v>
+      </c>
+      <c r="L119">
+        <v>1.5029999999999999</v>
+      </c>
+      <c r="M119">
+        <v>13.029</v>
+      </c>
+      <c r="N119">
+        <v>43.453000000000003</v>
+      </c>
+      <c r="O119" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>25</v>
+      </c>
+      <c r="B120" t="s">
+        <v>40</v>
+      </c>
+      <c r="C120" t="s">
+        <v>37</v>
+      </c>
+      <c r="D120">
+        <v>2021</v>
+      </c>
+      <c r="E120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F120">
+        <v>1</v>
+      </c>
+      <c r="G120" s="1">
+        <v>2</v>
+      </c>
+      <c r="H120" s="1">
+        <v>2</v>
+      </c>
+      <c r="I120" s="2">
+        <v>41.298000000000002</v>
+      </c>
+      <c r="J120">
+        <v>54.197000000000003</v>
+      </c>
+      <c r="K120">
+        <v>0</v>
+      </c>
+      <c r="L120">
+        <v>1.587</v>
+      </c>
+      <c r="M120">
+        <v>14.002000000000001</v>
+      </c>
+      <c r="N120">
+        <v>44.164999999999999</v>
+      </c>
+      <c r="O120" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>25</v>
+      </c>
+      <c r="B121" t="s">
+        <v>40</v>
+      </c>
+      <c r="C121" t="s">
+        <v>37</v>
+      </c>
+      <c r="D121">
+        <v>2021</v>
+      </c>
+      <c r="E121" t="s">
+        <v>10</v>
+      </c>
+      <c r="F121">
+        <v>1</v>
+      </c>
+      <c r="G121" s="1">
+        <v>2</v>
+      </c>
+      <c r="H121" s="1">
+        <v>2</v>
+      </c>
+      <c r="I121" s="2">
+        <v>40.991999999999997</v>
+      </c>
+      <c r="J121">
+        <v>55.234999999999999</v>
+      </c>
+      <c r="K121">
+        <v>0</v>
+      </c>
+      <c r="L121">
+        <v>1.5920000000000001</v>
+      </c>
+      <c r="M121">
+        <v>13.324999999999999</v>
+      </c>
+      <c r="N121">
+        <v>43.97</v>
+      </c>
+      <c r="O121" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>26</v>
+      </c>
+      <c r="B122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C122" t="s">
+        <v>37</v>
+      </c>
+      <c r="D122">
+        <v>2021</v>
+      </c>
+      <c r="E122" t="s">
+        <v>8</v>
+      </c>
+      <c r="F122">
+        <v>1</v>
+      </c>
+      <c r="G122" s="1">
+        <v>2</v>
+      </c>
+      <c r="H122" s="1">
+        <v>2</v>
+      </c>
+      <c r="I122" s="2">
+        <v>60.994</v>
+      </c>
+      <c r="J122">
+        <v>86.278999999999996</v>
+      </c>
+      <c r="K122">
+        <v>0</v>
+      </c>
+      <c r="L122">
+        <v>2.2080000000000002</v>
+      </c>
+      <c r="M122">
+        <v>6.1239999999999997</v>
+      </c>
+      <c r="N122">
+        <v>30.675999999999998</v>
+      </c>
+      <c r="O122" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>26</v>
+      </c>
+      <c r="B123" t="s">
+        <v>40</v>
+      </c>
+      <c r="C123" t="s">
+        <v>37</v>
+      </c>
+      <c r="D123">
+        <v>2021</v>
+      </c>
+      <c r="E123" t="s">
+        <v>9</v>
+      </c>
+      <c r="F123">
+        <v>1</v>
+      </c>
+      <c r="G123" s="1">
+        <v>2</v>
+      </c>
+      <c r="H123" s="1">
+        <v>2</v>
+      </c>
+      <c r="I123" s="2">
+        <v>61.234999999999999</v>
+      </c>
+      <c r="J123">
+        <v>86.991</v>
+      </c>
+      <c r="K123">
+        <v>0</v>
+      </c>
+      <c r="L123">
+        <v>2.3490000000000002</v>
+      </c>
+      <c r="M123">
+        <v>6.0279999999999996</v>
+      </c>
+      <c r="N123">
+        <v>34.521000000000001</v>
+      </c>
+      <c r="O123" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>26</v>
+      </c>
+      <c r="B124" t="s">
+        <v>40</v>
+      </c>
+      <c r="C124" t="s">
+        <v>37</v>
+      </c>
+      <c r="D124">
+        <v>2021</v>
+      </c>
+      <c r="E124" t="s">
+        <v>10</v>
+      </c>
+      <c r="F124">
+        <v>1</v>
+      </c>
+      <c r="G124" s="1">
+        <v>2</v>
+      </c>
+      <c r="H124" s="1">
+        <v>2</v>
+      </c>
+      <c r="I124" s="2">
+        <v>60.526000000000003</v>
+      </c>
+      <c r="J124">
+        <v>87.156000000000006</v>
+      </c>
+      <c r="K124">
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <v>2.5139999999999998</v>
+      </c>
+      <c r="M124">
+        <v>6.1890000000000001</v>
+      </c>
+      <c r="N124">
+        <v>31.222000000000001</v>
+      </c>
+      <c r="O124" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>27</v>
+      </c>
+      <c r="B125" t="s">
+        <v>40</v>
+      </c>
+      <c r="C125" t="s">
+        <v>37</v>
+      </c>
+      <c r="D125">
+        <v>2021</v>
+      </c>
+      <c r="E125" t="s">
+        <v>8</v>
+      </c>
+      <c r="F125">
+        <v>1</v>
+      </c>
+      <c r="G125" s="1">
+        <v>2</v>
+      </c>
+      <c r="H125" s="1">
+        <v>2</v>
+      </c>
+      <c r="I125" s="2">
+        <v>44.957999999999998</v>
+      </c>
+      <c r="J125">
+        <v>0</v>
+      </c>
+      <c r="K125">
+        <v>0</v>
+      </c>
+      <c r="L125">
+        <v>1.056</v>
+      </c>
+      <c r="M125">
+        <v>4.4139999999999997</v>
+      </c>
+      <c r="N125">
+        <v>49.459000000000003</v>
+      </c>
+      <c r="O125" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>27</v>
+      </c>
+      <c r="B126" t="s">
+        <v>40</v>
+      </c>
+      <c r="C126" t="s">
+        <v>37</v>
+      </c>
+      <c r="D126">
+        <v>2021</v>
+      </c>
+      <c r="E126" t="s">
+        <v>9</v>
+      </c>
+      <c r="F126">
+        <v>1</v>
+      </c>
+      <c r="G126" s="1">
+        <v>2</v>
+      </c>
+      <c r="H126" s="1">
+        <v>2</v>
+      </c>
+      <c r="I126" s="2">
+        <v>45.238999999999997</v>
+      </c>
+      <c r="J126">
+        <v>0</v>
+      </c>
+      <c r="K126">
+        <v>0</v>
+      </c>
+      <c r="L126">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="M126">
+        <v>5.23</v>
+      </c>
+      <c r="N126">
+        <v>55.238999999999997</v>
+      </c>
+      <c r="O126" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>27</v>
+      </c>
+      <c r="B127" t="s">
+        <v>40</v>
+      </c>
+      <c r="C127" t="s">
+        <v>37</v>
+      </c>
+      <c r="D127">
+        <v>2021</v>
+      </c>
+      <c r="E127" t="s">
+        <v>10</v>
+      </c>
+      <c r="F127">
+        <v>1</v>
+      </c>
+      <c r="G127" s="1">
+        <v>2</v>
+      </c>
+      <c r="H127" s="1">
+        <v>2</v>
+      </c>
+      <c r="I127" s="2">
+        <v>44.268000000000001</v>
+      </c>
+      <c r="J127">
+        <v>0</v>
+      </c>
+      <c r="K127">
+        <v>0</v>
+      </c>
+      <c r="L127">
+        <v>0.998</v>
+      </c>
+      <c r="M127">
+        <v>4.6870000000000003</v>
+      </c>
+      <c r="N127">
+        <v>52.686999999999998</v>
+      </c>
+      <c r="O127" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>28</v>
+      </c>
+      <c r="B128" t="s">
+        <v>40</v>
+      </c>
+      <c r="C128" t="s">
+        <v>37</v>
+      </c>
+      <c r="D128">
+        <v>2021</v>
+      </c>
+      <c r="E128" t="s">
+        <v>8</v>
+      </c>
+      <c r="F128">
+        <v>1</v>
+      </c>
+      <c r="G128" s="1">
+        <v>2</v>
+      </c>
+      <c r="H128" s="1">
+        <v>2</v>
+      </c>
+      <c r="I128" s="2">
+        <v>31.335000000000001</v>
+      </c>
+      <c r="J128">
+        <v>0</v>
+      </c>
+      <c r="K128">
+        <v>13.311</v>
+      </c>
+      <c r="L128">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="M128">
+        <v>2.456</v>
+      </c>
+      <c r="N128">
+        <v>14.066000000000001</v>
+      </c>
+      <c r="O128" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>28</v>
+      </c>
+      <c r="B129" t="s">
+        <v>40</v>
+      </c>
+      <c r="C129" t="s">
+        <v>37</v>
+      </c>
+      <c r="D129">
+        <v>2021</v>
+      </c>
+      <c r="E129" t="s">
+        <v>9</v>
+      </c>
+      <c r="F129">
+        <v>1</v>
+      </c>
+      <c r="G129" s="1">
+        <v>2</v>
+      </c>
+      <c r="H129" s="1">
+        <v>2</v>
+      </c>
+      <c r="I129" s="2">
+        <v>30.986999999999998</v>
+      </c>
+      <c r="J129">
+        <v>0</v>
+      </c>
+      <c r="K129">
+        <v>13.57</v>
+      </c>
+      <c r="L129">
+        <v>1.115</v>
+      </c>
+      <c r="M129">
+        <v>2.536</v>
+      </c>
+      <c r="N129">
+        <v>15.298</v>
+      </c>
+      <c r="O129" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>28</v>
+      </c>
+      <c r="B130" t="s">
+        <v>40</v>
+      </c>
+      <c r="C130" t="s">
+        <v>37</v>
+      </c>
+      <c r="D130">
+        <v>2021</v>
+      </c>
+      <c r="E130" t="s">
+        <v>10</v>
+      </c>
+      <c r="F130">
+        <v>1</v>
+      </c>
+      <c r="G130" s="1">
+        <v>2</v>
+      </c>
+      <c r="H130" s="1">
+        <v>2</v>
+      </c>
+      <c r="I130" s="2">
+        <v>35.670999999999999</v>
+      </c>
+      <c r="J130">
+        <v>0</v>
+      </c>
+      <c r="K130">
+        <v>15.09</v>
+      </c>
+      <c r="L130">
+        <v>1.097</v>
+      </c>
+      <c r="M130">
+        <v>2.6349999999999998</v>
+      </c>
+      <c r="N130">
+        <v>14.571</v>
+      </c>
+      <c r="O130" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>29</v>
+      </c>
+      <c r="B131" t="s">
+        <v>40</v>
+      </c>
+      <c r="C131" t="s">
+        <v>37</v>
+      </c>
+      <c r="D131">
+        <v>2021</v>
+      </c>
+      <c r="E131" t="s">
+        <v>8</v>
+      </c>
+      <c r="F131">
+        <v>1</v>
+      </c>
+      <c r="G131" s="1">
+        <v>2</v>
+      </c>
+      <c r="H131" s="1">
+        <v>2</v>
+      </c>
+      <c r="I131" s="2">
+        <v>0</v>
+      </c>
+      <c r="J131">
+        <v>61.268000000000001</v>
+      </c>
+      <c r="K131">
+        <v>0</v>
+      </c>
+      <c r="L131">
+        <v>1.0529999999999999</v>
+      </c>
+      <c r="M131">
+        <v>4.9359999999999999</v>
+      </c>
+      <c r="N131">
+        <v>71.123999999999995</v>
+      </c>
+      <c r="O131" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>29</v>
+      </c>
+      <c r="B132" t="s">
+        <v>40</v>
+      </c>
+      <c r="C132" t="s">
+        <v>37</v>
+      </c>
+      <c r="D132">
+        <v>2021</v>
+      </c>
+      <c r="E132" t="s">
+        <v>9</v>
+      </c>
+      <c r="F132">
+        <v>1</v>
+      </c>
+      <c r="G132" s="1">
+        <v>2</v>
+      </c>
+      <c r="H132" s="1">
+        <v>2</v>
+      </c>
+      <c r="I132" s="2">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="J132">
+        <v>63.517000000000003</v>
+      </c>
+      <c r="K132">
+        <v>0</v>
+      </c>
+      <c r="L132">
+        <v>1.125</v>
+      </c>
+      <c r="M132">
+        <v>5.1230000000000002</v>
+      </c>
+      <c r="N132">
+        <v>70.980999999999995</v>
+      </c>
+      <c r="O132" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>29</v>
+      </c>
+      <c r="B133" t="s">
+        <v>40</v>
+      </c>
+      <c r="C133" t="s">
+        <v>37</v>
+      </c>
+      <c r="D133">
+        <v>2021</v>
+      </c>
+      <c r="E133" t="s">
+        <v>10</v>
+      </c>
+      <c r="F133">
+        <v>1</v>
+      </c>
+      <c r="G133" s="1">
+        <v>2</v>
+      </c>
+      <c r="H133" s="1">
+        <v>2</v>
+      </c>
+      <c r="I133" s="2">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="J133">
+        <v>60.978000000000002</v>
+      </c>
+      <c r="K133">
+        <v>0</v>
+      </c>
+      <c r="L133">
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="M133">
+        <v>4.992</v>
+      </c>
+      <c r="N133">
+        <v>71.960999999999999</v>
+      </c>
+      <c r="O133" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>30</v>
+      </c>
+      <c r="B134" t="s">
+        <v>40</v>
+      </c>
+      <c r="C134" t="s">
+        <v>37</v>
+      </c>
+      <c r="D134">
+        <v>2021</v>
+      </c>
+      <c r="E134" t="s">
+        <v>8</v>
+      </c>
+      <c r="F134">
+        <v>1</v>
+      </c>
+      <c r="G134" s="1">
+        <v>2</v>
+      </c>
+      <c r="H134" s="1">
+        <v>2</v>
+      </c>
+      <c r="I134" s="2">
+        <v>46.893000000000001</v>
+      </c>
+      <c r="J134">
+        <v>68.143000000000001</v>
+      </c>
+      <c r="K134">
+        <v>0</v>
+      </c>
+      <c r="L134">
+        <v>1.125</v>
+      </c>
+      <c r="M134">
+        <v>6.05</v>
+      </c>
+      <c r="N134">
+        <v>26.8</v>
+      </c>
+      <c r="O134" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>30</v>
+      </c>
+      <c r="B135" t="s">
+        <v>40</v>
+      </c>
+      <c r="C135" t="s">
+        <v>37</v>
+      </c>
+      <c r="D135">
+        <v>2021</v>
+      </c>
+      <c r="E135" t="s">
+        <v>9</v>
+      </c>
+      <c r="F135">
+        <v>1</v>
+      </c>
+      <c r="G135" s="1">
+        <v>2</v>
+      </c>
+      <c r="H135" s="1">
+        <v>2</v>
+      </c>
+      <c r="I135" s="2">
+        <v>47.366999999999997</v>
+      </c>
+      <c r="J135">
+        <v>70.256</v>
+      </c>
+      <c r="K135">
+        <v>0</v>
+      </c>
+      <c r="L135">
+        <v>1.2350000000000001</v>
+      </c>
+      <c r="M135">
+        <v>6.24</v>
+      </c>
+      <c r="N135">
+        <v>28.611999999999998</v>
+      </c>
+      <c r="O135" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>30</v>
+      </c>
+      <c r="B136" t="s">
+        <v>40</v>
+      </c>
+      <c r="C136" t="s">
+        <v>37</v>
+      </c>
+      <c r="D136">
+        <v>2021</v>
+      </c>
+      <c r="E136" t="s">
+        <v>10</v>
+      </c>
+      <c r="F136">
+        <v>1</v>
+      </c>
+      <c r="G136" s="1">
+        <v>2</v>
+      </c>
+      <c r="H136" s="1">
+        <v>2</v>
+      </c>
+      <c r="I136" s="2">
+        <v>46.094999999999999</v>
+      </c>
+      <c r="J136">
+        <v>69.337000000000003</v>
+      </c>
+      <c r="K136">
+        <v>0</v>
+      </c>
+      <c r="L136">
+        <v>1.1919999999999999</v>
+      </c>
+      <c r="M136">
+        <v>7.05</v>
+      </c>
+      <c r="N136">
+        <v>26.15</v>
+      </c>
+      <c r="O136" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>